<commit_message>
added input handle func (#2)
</commit_message>
<xml_diff>
--- a/Lab - Testing/Testing.xlsx
+++ b/Lab - Testing/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/C++Projects/CS1B/Lab - Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C991968D-FB90-A44D-8C5B-EE1C380ADB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE449B-4B5B-8348-97AF-2DDE834C98B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{3D8F6425-9EB6-DF45-B2B1-4AE88F52F0E0}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Black Box</t>
   </si>
   <si>
-    <t>3 4</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -73,13 +70,16 @@
     <t>White Box</t>
   </si>
   <si>
-    <t>0 0</t>
-  </si>
-  <si>
     <t>Boundary/Expected</t>
   </si>
   <si>
-    <t>16 4</t>
+    <t>0, 0</t>
+  </si>
+  <si>
+    <t>4, 3</t>
+  </si>
+  <si>
+    <t>4, 16</t>
   </si>
 </sst>
 </file>
@@ -103,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,12 +111,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +452,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,83 +463,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>